<commit_message>
First working implementation of 4-SF
</commit_message>
<xml_diff>
--- a/forms/Form-3AR-multiple.xlsx
+++ b/forms/Form-3AR-multiple.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD518AD6-202B-4BD8-B656-8B08B417633A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA93F59-81CB-412E-812E-7A2879025811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="+fpbANi5+/yFWHPxzEqaReNDzPx7npT1czOQfFrctV9jGFhmw0Jnw7c42DyBMqUzdexUCp19VjI1OGlWew7xXA==" workbookSaltValue="bMmY3IsF10EHABvsu//kNQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
+    <workbookView xWindow="32715" yWindow="3645" windowWidth="21600" windowHeight="11295" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -1966,7 +1966,7 @@
       <c r="BP4" s="45"/>
       <c r="BQ4" s="46"/>
     </row>
-    <row r="5" spans="2:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:69" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="67" t="s">
         <v>9</v>
       </c>
@@ -5576,7 +5576,7 @@
       <c r="S1048576" s="53"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="UJ/l6Dp57n5EXak/I0C4ijeZDdMtsb5EmZBHDh8WfNldw4fQPIh9ATxAd9pzxptKu/+atnNtoQ/HyMiCv/Uurg==" saltValue="Zs3XDgbzVESCbltWiNZuWQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="D1a8kN8ZiG7GMvhYHXpgZJ4eGgHFaIGoW+hRc2Jznz349uAvHPHL5jYmIK9r2sdhczfvJOVXq60jYGlDSMHPsA==" saltValue="LjjV0cpjndXxrJVGyan5Kw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="T3:BQ3"/>
     <mergeCell ref="B4:F4"/>
@@ -5585,11 +5585,8 @@
     <mergeCell ref="M4:R4"/>
     <mergeCell ref="B2:R3"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S4:S5 M5 O5 Q5 J5 K5 C5 E5:I5" xr:uid="{B1699078-27D6-472D-B920-0B9DAA1EA97D}">
-      <formula1>"&lt;0&gt;0"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5" xr:uid="{87FE9B35-DFCC-43D6-898C-FAD86BBA51D1}">
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S4:S5 M5 O5 Q5 C5:K5" xr:uid="{B1699078-27D6-472D-B920-0B9DAA1EA97D}">
       <formula1>"&lt;0&gt;0"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>